<commit_message>
Updated Test Case File 2.0
</commit_message>
<xml_diff>
--- a/Testing/Test Cases.xlsx
+++ b/Testing/Test Cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\University Work\CT4003 Programming and Software Development\Semester Two\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -126,6 +126,69 @@
   </si>
   <si>
     <t>RJ008</t>
+  </si>
+  <si>
+    <t>RA001/N</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>RA002/N</t>
+  </si>
+  <si>
+    <t>RA003/N</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>RJ004/N</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>RJ005/N</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>RJ006/N</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>RJ007/N</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Severity (Major, Minor)</t>
+  </si>
+  <si>
+    <t>Initiate the system, move the Arduino board from its original location</t>
+  </si>
+  <si>
+    <t>The Arduino would pick up the movement and send a seven to the Java code to initiate the breach email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Arduino board would </t>
+  </si>
+  <si>
+    <t>Initiate the system, and place a object in the path of the ultrasonic sensor</t>
   </si>
 </sst>
 </file>
@@ -149,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +222,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,11 +256,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K11"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,15 +557,17 @@
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="95.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,95 +596,233 @@
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E10" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D18" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>